<commit_message>
added ability for user to set days off
User can now enter days they missed from work and they won't be written into the schedule.
</commit_message>
<xml_diff>
--- a/paysheet.xlsx
+++ b/paysheet.xlsx
@@ -352,7 +352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -865,27 +865,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>F70</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>W60</t>
+          <t>W67</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -897,12 +897,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>W61</t>
+          <t>W52</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -912,125 +912,125 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>W71</t>
+          <t>W49</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>W49</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W57</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4/10</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W75</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>F70</t>
+          <t>W48</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>W67</t>
+          <t>W45</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1040,108 +1040,108 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>W52</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/15</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>W49</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W60</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4/12</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W61</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>W57</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>W75</t>
+          <t>W71</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1153,12 +1153,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>W48</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1168,24 +1168,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>W45</t>
+          <t>W49</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4/15</t>
+          <t>4/17</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1217,27 +1217,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>F70</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>W60</t>
+          <t>W67</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1249,12 +1249,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>W61</t>
+          <t>W52</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1264,125 +1264,125 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>W71</t>
+          <t>W49</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/19</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>W49</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W57</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4/17</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W75</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>F70</t>
+          <t>W48</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>W67</t>
+          <t>W45</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1392,108 +1392,108 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>W52</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/22</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>W49</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W60</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4/19</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W61</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>W57</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>W75</t>
+          <t>W71</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1505,12 +1505,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>W48</t>
+          <t>w66</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1520,24 +1520,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>W45</t>
+          <t>W49</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>4/24</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1569,27 +1569,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>F70</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>W60</t>
+          <t>W67</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1601,12 +1601,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>W61</t>
+          <t>W52</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1616,125 +1616,125 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>w46</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>W71</t>
+          <t>W49</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>w66</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/26</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>W49</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>.5 hour</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W57</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Homework period</t>
+          <t>W75</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>.5 hour</t>
+          <t>1 hour</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>F70</t>
+          <t>W48</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>1 hour</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>W67</t>
+          <t>W45</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1744,175 +1744,32 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>W52</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1 hour</t>
+          <t>.5 hour</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>4/26</t>
+          <t>4/29</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>w46</t>
+          <t>Homework period</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
-        <is>
-          <t>1 hour</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>4/26</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>W49</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2 hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>4/26</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>.5 hour</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>4/26</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>.5 hour</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>W57</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>1 hour</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>W75</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>1 hour</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>W48</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>1 hour</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>W45</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>1 hour</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>.5 hour</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>4/29</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>

</xml_diff>

<commit_message>
Cleaned up sheet layout
Title now sits closer to center, still depends on size of users name

There is a now a blank space between the two classes worth of into written across each row.
</commit_message>
<xml_diff>
--- a/paysheet.xlsx
+++ b/paysheet.xlsx
@@ -352,7 +352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -361,13 +361,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="2" min="2" width="20"/>
-    <col customWidth="1" max="6" min="6" width="20"/>
+    <col customWidth="1" max="7" min="7" width="20"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ginos Paysheet for 04/2019</t>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ginos Paysheet:04/2019</t>
         </is>
       </c>
     </row>
@@ -393,22 +393,22 @@
           <t>Signature</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Class name</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Length</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
@@ -430,17 +430,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>4/1</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>W75</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -462,17 +462,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>4/1</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>W45</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -494,17 +494,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>4/1</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -526,17 +526,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>4/3</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>W60</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -558,17 +558,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>4/3</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>PE</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -590,17 +590,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>4/3</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>w66</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -622,17 +622,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>4/3</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -654,17 +654,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>4/5</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>F70</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>2 hours</t>
         </is>
@@ -686,17 +686,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>4/5</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>W52</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -718,17 +718,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>4/5</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>W49</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>2 hours</t>
         </is>
@@ -750,17 +750,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>4/5</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -782,17 +782,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>4/8</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>W75</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -814,17 +814,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>4/8</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>W45</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -846,17 +846,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>4/8</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -878,17 +878,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>4/12</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>W67</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -910,17 +910,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>4/12</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>w46</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -942,17 +942,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>4/12</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G20" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -974,17 +974,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>4/15</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>W57</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1006,17 +1006,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>4/15</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>W48</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1038,17 +1038,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>4/15</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1070,17 +1070,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>4/17</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>PE</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1102,17 +1102,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>4/17</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>W61</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1134,17 +1134,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>4/17</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>W71</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1166,17 +1166,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>4/17</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>W49</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>2 hours</t>
         </is>
@@ -1198,17 +1198,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>4/17</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1230,17 +1230,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>4/19</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>W67</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1262,17 +1262,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>4/19</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>w46</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1294,17 +1294,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>4/19</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1326,17 +1326,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>4/22</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>W57</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1358,17 +1358,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>4/22</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>W48</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1390,17 +1390,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>4/22</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G34" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1422,17 +1422,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>4/24</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>PE</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1454,17 +1454,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>4/24</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>W61</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1486,17 +1486,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>4/24</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>W71</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1518,17 +1518,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>4/24</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>W49</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>2 hours</t>
         </is>
@@ -1550,17 +1550,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>4/24</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G39" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1582,17 +1582,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>4/26</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>W67</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1614,17 +1614,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>4/26</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>w46</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1646,17 +1646,17 @@
           <t>2 hours</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>4/26</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G42" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1678,17 +1678,17 @@
           <t>.5 hour</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>4/29</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>W57</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1710,17 +1710,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>4/29</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>W48</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>1 hour</t>
         </is>
@@ -1742,17 +1742,17 @@
           <t>1 hour</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>4/29</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Homework period</t>
-        </is>
-      </c>
       <c r="G45" t="inlineStr">
+        <is>
+          <t>Homework period</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
         <is>
           <t>.5 hour</t>
         </is>
@@ -1777,7 +1777,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:J2"/>
+    <mergeCell ref="C1:G2"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved formatting + adds ending message
Excel sheet formatting now improved via changing cell sizes.

A message now displays at the end telling the user if the process was a sucess or the most likely error and how to fix it if it wasn't.
</commit_message>
<xml_diff>
--- a/paysheet.xlsx
+++ b/paysheet.xlsx
@@ -29,7 +29,7 @@
       <name val="Times New Roman"/>
       <b val="1"/>
       <i val="1"/>
-      <sz val="25"/>
+      <sz val="20"/>
     </font>
   </fonts>
   <fills count="2">
@@ -360,8 +360,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="20"/>
-    <col customWidth="1" max="7" min="7" width="20"/>
+    <col customWidth="1" max="1" min="1" width="6"/>
+    <col customWidth="1" max="2" min="2" width="17"/>
+    <col customWidth="1" max="5" min="5" width="5"/>
+    <col customWidth="1" max="6" min="6" width="6"/>
+    <col customWidth="1" max="7" min="7" width="17"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>